<commit_message>
edit Game and tracks Changes Test
</commit_message>
<xml_diff>
--- a/Phase 3/ST-COMM-Testing-phase3/editGame.xlsx
+++ b/Phase 3/ST-COMM-Testing-phase3/editGame.xlsx
@@ -19,12 +19,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>Jack</t>
   </si>
   <si>
     <t>123C456</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Add2Numbers</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>5+11=16</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>2+19=20</t>
+  </si>
+  <si>
+    <t>T/F</t>
+  </si>
+  <si>
+    <t>MCQ</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>12+1=?</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
 </sst>
 </file>
@@ -343,20 +391,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>